<commit_message>
Upload Files A1#111#NAMURSRLXX - Namur srl - GLPX - 1.0
Upload Files per Mancato accreditamento A1#111#NAMURSRLXX - Namur srl - GLPX - 1.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#NAMURSRLXX/Namur srl/GLPX/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#NAMURSRLXX/Namur srl/GLPX/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\it-fse-accreditamento\GATEWAY\A1#111#NAMURSRLXX\Namur srl\GLPX\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DE1745-3DB6-467B-80FF-650F3F6B45F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC954E-DC48-4E6F-BB60-9F8DD70157D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30960" yWindow="1965" windowWidth="24225" windowHeight="13770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="571">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1676,9 +1676,6 @@
     <t>c8fab8ceca801404</t>
   </si>
   <si>
-    <t>92dfb0d60b01dcf5</t>
-  </si>
-  <si>
     <t>f79a0beae35cc259</t>
   </si>
   <si>
@@ -1734,9 +1731,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.7561f0980b0d44a9c3c6de232cb035c196121f4b214526872f0d0326e245ed6c.1c8b4c74d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6bb8cdc6c82db4e1d96aa426379a660bd55e46b6018529337d90c49e72a27127.140bf14a2f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.7561f0980b0d44a9c3c6de232cb035c196121f4b214526872f0d0326e245ed6c.a1dd7239ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
@@ -2006,6 +2000,15 @@
   </si>
   <si>
     <t>L’errore è registrato in un log applicativo. il medico ha 2 opzioni: A) eseguire  una nuova chiamata al servizio di validazione  B) firmare  il referto  privo della validazione  così da poter consegnare al paziente il referto. I referti da validare , sono evidenziati in un pannello al medico  in modo che possa procedere alla validazione</t>
+  </si>
+  <si>
+    <t>2024-11-07T08:18:37Z</t>
+  </si>
+  <si>
+    <t>f9487499a218b831</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6bb8cdc6c82db4e1d96aa426379a660bd55e46b6018529337d90c49e72a27127.7d0daf3664^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4023,10 +4026,10 @@
   <dimension ref="A1:W809"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J231" sqref="J231"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4275,52 +4278,52 @@
         <v>461</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J9" s="17" t="s">
+        <v>498</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>502</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="N9" s="17" t="s">
         <v>503</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="O9" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="P9" s="17" t="s">
         <v>505</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="Q9" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="R9" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="Q9" s="17" t="s">
+      <c r="S9" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="R9" s="17" t="s">
+      <c r="T9" s="17" t="s">
         <v>509</v>
       </c>
-      <c r="S9" s="17" t="s">
+      <c r="U9" s="29" t="s">
         <v>510</v>
       </c>
-      <c r="T9" s="17" t="s">
+      <c r="V9" s="17" t="s">
         <v>511</v>
       </c>
-      <c r="U9" s="29" t="s">
+      <c r="W9" s="44" t="s">
         <v>512</v>
       </c>
-      <c r="V9" s="17" t="s">
-        <v>513</v>
-      </c>
-      <c r="W9" s="44" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>1</v>
       </c>
@@ -4346,38 +4349,38 @@
         <v>462</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
       <c r="M10" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O10" s="34"/>
       <c r="P10" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q10" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R10" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S10" s="34"/>
       <c r="T10" s="34"/>
       <c r="U10" s="31"/>
       <c r="V10" s="39"/>
       <c r="W10" s="45" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>2</v>
       </c>
@@ -4403,38 +4406,38 @@
         <v>463</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
       <c r="M11" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N11" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O11" s="34"/>
       <c r="P11" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q11" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R11" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S11" s="34"/>
       <c r="T11" s="34"/>
       <c r="U11" s="31"/>
       <c r="V11" s="39"/>
       <c r="W11" s="45" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>3</v>
       </c>
@@ -4460,38 +4463,38 @@
         <v>464</v>
       </c>
       <c r="I12" s="30" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
       <c r="M12" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N12" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O12" s="34"/>
       <c r="P12" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q12" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R12" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S12" s="34"/>
       <c r="T12" s="34"/>
       <c r="U12" s="31"/>
       <c r="V12" s="39"/>
       <c r="W12" s="45" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -4508,47 +4511,47 @@
         <v>258</v>
       </c>
       <c r="F13" s="25">
-        <v>45593</v>
-      </c>
-      <c r="G13" s="30">
-        <v>45593.476631944402</v>
+        <v>45603</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>568</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>465</v>
+        <v>569</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>485</v>
+        <v>570</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
       <c r="M13" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O13" s="34"/>
       <c r="P13" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R13" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S13" s="34"/>
       <c r="T13" s="34"/>
       <c r="U13" s="31"/>
       <c r="V13" s="39"/>
       <c r="W13" s="45" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>5</v>
       </c>
@@ -4571,38 +4574,38 @@
         <v>45593.476643518501</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O14" s="34"/>
       <c r="P14" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q14" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R14" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S14" s="34"/>
       <c r="T14" s="34"/>
       <c r="U14" s="31"/>
       <c r="V14" s="39"/>
       <c r="W14" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4632,7 +4635,7 @@
       <c r="N15" s="34"/>
       <c r="O15" s="34"/>
       <c r="P15" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q15" s="34"/>
       <c r="R15" s="34"/>
@@ -4641,7 +4644,7 @@
       <c r="U15" s="31"/>
       <c r="V15" s="39"/>
       <c r="W15" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4678,7 +4681,7 @@
       <c r="U16" s="31"/>
       <c r="V16" s="39"/>
       <c r="W16" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4715,7 +4718,7 @@
       <c r="U17" s="31"/>
       <c r="V17" s="39"/>
       <c r="W17" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4752,7 +4755,7 @@
       <c r="U18" s="31"/>
       <c r="V18" s="39"/>
       <c r="W18" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4789,7 +4792,7 @@
       <c r="U19" s="31"/>
       <c r="V19" s="39"/>
       <c r="W19" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4826,7 +4829,7 @@
       <c r="U20" s="31"/>
       <c r="V20" s="39"/>
       <c r="W20" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4863,7 +4866,7 @@
       <c r="U21" s="31"/>
       <c r="V21" s="39"/>
       <c r="W21" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4900,7 +4903,7 @@
       <c r="U22" s="31"/>
       <c r="V22" s="39"/>
       <c r="W22" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4937,7 +4940,7 @@
       <c r="U23" s="31"/>
       <c r="V23" s="39"/>
       <c r="W23" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -4974,7 +4977,7 @@
       <c r="U24" s="31"/>
       <c r="V24" s="39"/>
       <c r="W24" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5011,7 +5014,7 @@
       <c r="U25" s="31"/>
       <c r="V25" s="39"/>
       <c r="W25" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5048,7 +5051,7 @@
       <c r="U26" s="31"/>
       <c r="V26" s="39"/>
       <c r="W26" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5085,7 +5088,7 @@
       <c r="U27" s="31"/>
       <c r="V27" s="39"/>
       <c r="W27" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5122,7 +5125,7 @@
       <c r="U28" s="31"/>
       <c r="V28" s="39"/>
       <c r="W28" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5159,7 +5162,7 @@
       <c r="U29" s="31"/>
       <c r="V29" s="39"/>
       <c r="W29" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5196,10 +5199,10 @@
       <c r="U30" s="31"/>
       <c r="V30" s="39"/>
       <c r="W30" s="45" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
         <v>28</v>
       </c>
@@ -5222,42 +5225,42 @@
         <v>450</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I31" s="30" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="J31" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
       <c r="M31" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N31" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O31" s="58" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="P31" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q31" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R31" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S31" s="34" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T31" s="34"/>
       <c r="U31" s="31"/>
       <c r="V31" s="39"/>
       <c r="W31" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5294,7 +5297,7 @@
       <c r="U32" s="31"/>
       <c r="V32" s="39"/>
       <c r="W32" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5331,7 +5334,7 @@
       <c r="U33" s="31"/>
       <c r="V33" s="39"/>
       <c r="W33" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5368,7 +5371,7 @@
       <c r="U34" s="31"/>
       <c r="V34" s="39"/>
       <c r="W34" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5405,7 +5408,7 @@
       <c r="U35" s="31"/>
       <c r="V35" s="39"/>
       <c r="W35" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5442,7 +5445,7 @@
       <c r="U36" s="31"/>
       <c r="V36" s="39"/>
       <c r="W36" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5479,7 +5482,7 @@
       <c r="U37" s="31"/>
       <c r="V37" s="39"/>
       <c r="W37" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5516,10 +5519,10 @@
       <c r="U38" s="31"/>
       <c r="V38" s="39"/>
       <c r="W38" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
         <v>36</v>
       </c>
@@ -5542,42 +5545,42 @@
         <v>451</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I39" s="30" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="J39" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
       <c r="M39" s="34" t="s">
+        <v>551</v>
+      </c>
+      <c r="N39" s="34" t="s">
+        <v>499</v>
+      </c>
+      <c r="O39" s="58" t="s">
         <v>553</v>
       </c>
-      <c r="N39" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="O39" s="58" t="s">
-        <v>555</v>
-      </c>
       <c r="P39" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q39" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R39" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S39" s="34" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T39" s="34"/>
       <c r="U39" s="31"/>
       <c r="V39" s="39"/>
       <c r="W39" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5614,7 +5617,7 @@
       <c r="U40" s="31"/>
       <c r="V40" s="39"/>
       <c r="W40" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5651,7 +5654,7 @@
       <c r="U41" s="31"/>
       <c r="V41" s="39"/>
       <c r="W41" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5688,7 +5691,7 @@
       <c r="U42" s="31"/>
       <c r="V42" s="39"/>
       <c r="W42" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5725,7 +5728,7 @@
       <c r="U43" s="31"/>
       <c r="V43" s="39"/>
       <c r="W43" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="44" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5762,7 +5765,7 @@
       <c r="U44" s="31"/>
       <c r="V44" s="39"/>
       <c r="W44" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5799,7 +5802,7 @@
       <c r="U45" s="31"/>
       <c r="V45" s="39"/>
       <c r="W45" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="46" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5836,7 +5839,7 @@
       <c r="U46" s="31"/>
       <c r="V46" s="39"/>
       <c r="W46" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5860,38 +5863,38 @@
       <c r="H47" s="30"/>
       <c r="I47" s="30"/>
       <c r="J47" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K47" s="34"/>
       <c r="L47" s="34"/>
       <c r="M47" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N47" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O47" s="34" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="P47" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q47" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R47" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S47" s="34" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="T47" s="34"/>
       <c r="U47" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V47" s="39"/>
       <c r="W47" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5926,11 +5929,11 @@
       <c r="S48" s="34"/>
       <c r="T48" s="34"/>
       <c r="U48" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V48" s="39"/>
       <c r="W48" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="49" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5965,11 +5968,11 @@
       <c r="S49" s="34"/>
       <c r="T49" s="34"/>
       <c r="U49" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V49" s="39"/>
       <c r="W49" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6004,11 +6007,11 @@
       <c r="S50" s="34"/>
       <c r="T50" s="34"/>
       <c r="U50" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V50" s="39"/>
       <c r="W50" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6043,11 +6046,11 @@
       <c r="S51" s="34"/>
       <c r="T51" s="34"/>
       <c r="U51" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V51" s="39"/>
       <c r="W51" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="52" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6082,11 +6085,11 @@
       <c r="S52" s="34"/>
       <c r="T52" s="34"/>
       <c r="U52" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V52" s="39"/>
       <c r="W52" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="53" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6121,11 +6124,11 @@
       <c r="S53" s="34"/>
       <c r="T53" s="34"/>
       <c r="U53" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V53" s="39"/>
       <c r="W53" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="54" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6160,14 +6163,14 @@
       <c r="S54" s="34"/>
       <c r="T54" s="34"/>
       <c r="U54" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V54" s="39"/>
       <c r="W54" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
         <v>52</v>
       </c>
@@ -6190,45 +6193,45 @@
         <v>452</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I55" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J55" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K55" s="34"/>
       <c r="L55" s="34"/>
       <c r="M55" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N55" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O55" s="58" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="P55" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q55" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R55" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S55" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T55" s="34"/>
       <c r="U55" s="31"/>
       <c r="V55" s="39"/>
       <c r="W55" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
         <v>53</v>
       </c>
@@ -6251,45 +6254,45 @@
         <v>453</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I56" s="30" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J56" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K56" s="34"/>
       <c r="L56" s="34"/>
       <c r="M56" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N56" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O56" s="58" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="P56" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q56" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R56" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S56" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T56" s="34"/>
       <c r="U56" s="31"/>
       <c r="V56" s="39"/>
       <c r="W56" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
         <v>54</v>
       </c>
@@ -6312,45 +6315,45 @@
         <v>453</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I57" s="30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="J57" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K57" s="34"/>
       <c r="L57" s="34"/>
       <c r="M57" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N57" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O57" s="58" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="P57" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q57" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R57" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S57" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T57" s="34"/>
       <c r="U57" s="31"/>
       <c r="V57" s="39"/>
       <c r="W57" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
         <v>55</v>
       </c>
@@ -6373,45 +6376,45 @@
         <v>454</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I58" s="30" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J58" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K58" s="34"/>
       <c r="L58" s="34"/>
       <c r="M58" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N58" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O58" s="58" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="P58" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q58" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R58" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S58" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T58" s="34"/>
       <c r="U58" s="31"/>
       <c r="V58" s="39"/>
       <c r="W58" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
         <v>56</v>
       </c>
@@ -6434,45 +6437,45 @@
         <v>455</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I59" s="30" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="J59" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K59" s="34"/>
       <c r="L59" s="34"/>
       <c r="M59" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N59" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O59" s="58" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="P59" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q59" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R59" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S59" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T59" s="34"/>
       <c r="U59" s="31"/>
       <c r="V59" s="39"/>
       <c r="W59" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
         <v>57</v>
       </c>
@@ -6495,45 +6498,45 @@
         <v>456</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I60" s="30" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J60" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K60" s="34"/>
       <c r="L60" s="34"/>
       <c r="M60" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N60" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O60" s="58" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="P60" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q60" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R60" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S60" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T60" s="34"/>
       <c r="U60" s="31"/>
       <c r="V60" s="39"/>
       <c r="W60" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
         <v>58</v>
       </c>
@@ -6556,45 +6559,45 @@
         <v>457</v>
       </c>
       <c r="H61" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I61" s="30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="J61" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K61" s="34"/>
       <c r="L61" s="34"/>
       <c r="M61" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N61" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O61" s="58" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="P61" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q61" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R61" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S61" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T61" s="34"/>
       <c r="U61" s="31"/>
       <c r="V61" s="39"/>
       <c r="W61" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="62" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
         <v>59</v>
       </c>
@@ -6617,45 +6620,45 @@
         <v>458</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I62" s="30" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J62" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K62" s="34"/>
       <c r="L62" s="34"/>
       <c r="M62" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N62" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O62" s="58" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="P62" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q62" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R62" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S62" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T62" s="34"/>
       <c r="U62" s="31"/>
       <c r="V62" s="39"/>
       <c r="W62" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="63" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
         <v>60</v>
       </c>
@@ -6678,45 +6681,45 @@
         <v>458</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I63" s="30" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="J63" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K63" s="34"/>
       <c r="L63" s="34"/>
       <c r="M63" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N63" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O63" s="58" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="P63" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q63" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R63" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S63" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T63" s="34"/>
       <c r="U63" s="31"/>
       <c r="V63" s="39"/>
       <c r="W63" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="64" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
         <v>61</v>
       </c>
@@ -6739,45 +6742,45 @@
         <v>459</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I64" s="30" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J64" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K64" s="34"/>
       <c r="L64" s="34"/>
       <c r="M64" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N64" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O64" s="58" t="s">
+        <v>564</v>
+      </c>
+      <c r="P64" s="34" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q64" s="34" t="s">
+        <v>551</v>
+      </c>
+      <c r="R64" s="34" t="s">
+        <v>499</v>
+      </c>
+      <c r="S64" s="58" t="s">
         <v>566</v>
-      </c>
-      <c r="P64" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="Q64" s="34" t="s">
-        <v>553</v>
-      </c>
-      <c r="R64" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="S64" s="58" t="s">
-        <v>568</v>
       </c>
       <c r="T64" s="34"/>
       <c r="U64" s="31"/>
       <c r="V64" s="39"/>
       <c r="W64" s="45" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="65" spans="1:23" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <v>62</v>
       </c>
@@ -6800,42 +6803,42 @@
         <v>460</v>
       </c>
       <c r="H65" s="30" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I65" s="30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="J65" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K65" s="34"/>
       <c r="L65" s="34"/>
       <c r="M65" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N65" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O65" s="58" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="P65" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q65" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R65" s="34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S65" s="58" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T65" s="34"/>
       <c r="U65" s="31"/>
       <c r="V65" s="39"/>
       <c r="W65" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="66" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6872,7 +6875,7 @@
       <c r="U66" s="31"/>
       <c r="V66" s="39"/>
       <c r="W66" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="67" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6909,7 +6912,7 @@
       <c r="U67" s="31"/>
       <c r="V67" s="39"/>
       <c r="W67" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="68" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6946,7 +6949,7 @@
       <c r="U68" s="31"/>
       <c r="V68" s="39"/>
       <c r="W68" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="69" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -6983,7 +6986,7 @@
       <c r="U69" s="31"/>
       <c r="V69" s="39"/>
       <c r="W69" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="70" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7020,7 +7023,7 @@
       <c r="U70" s="31"/>
       <c r="V70" s="39"/>
       <c r="W70" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="71" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7057,7 +7060,7 @@
       <c r="U71" s="31"/>
       <c r="V71" s="39"/>
       <c r="W71" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="72" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7094,7 +7097,7 @@
       <c r="U72" s="31"/>
       <c r="V72" s="39"/>
       <c r="W72" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="73" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7131,7 +7134,7 @@
       <c r="U73" s="31"/>
       <c r="V73" s="39"/>
       <c r="W73" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="74" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7168,7 +7171,7 @@
       <c r="U74" s="31"/>
       <c r="V74" s="39"/>
       <c r="W74" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="75" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7205,7 +7208,7 @@
       <c r="U75" s="31"/>
       <c r="V75" s="39"/>
       <c r="W75" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="76" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7242,7 +7245,7 @@
       <c r="U76" s="31"/>
       <c r="V76" s="39"/>
       <c r="W76" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="77" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7279,7 +7282,7 @@
       <c r="U77" s="31"/>
       <c r="V77" s="39"/>
       <c r="W77" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="78" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7316,7 +7319,7 @@
       <c r="U78" s="31"/>
       <c r="V78" s="39"/>
       <c r="W78" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="79" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7353,7 +7356,7 @@
       <c r="U79" s="31"/>
       <c r="V79" s="39"/>
       <c r="W79" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="80" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7390,7 +7393,7 @@
       <c r="U80" s="31"/>
       <c r="V80" s="39"/>
       <c r="W80" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="81" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7427,7 +7430,7 @@
       <c r="U81" s="31"/>
       <c r="V81" s="39"/>
       <c r="W81" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="82" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7464,7 +7467,7 @@
       <c r="U82" s="31"/>
       <c r="V82" s="39"/>
       <c r="W82" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="83" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7501,7 +7504,7 @@
       <c r="U83" s="31"/>
       <c r="V83" s="39"/>
       <c r="W83" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="84" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7538,7 +7541,7 @@
       <c r="U84" s="31"/>
       <c r="V84" s="39"/>
       <c r="W84" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="85" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7575,7 +7578,7 @@
       <c r="U85" s="31"/>
       <c r="V85" s="39"/>
       <c r="W85" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="86" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7612,7 +7615,7 @@
       <c r="U86" s="31"/>
       <c r="V86" s="39"/>
       <c r="W86" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="87" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7649,7 +7652,7 @@
       <c r="U87" s="31"/>
       <c r="V87" s="39"/>
       <c r="W87" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="88" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7686,7 +7689,7 @@
       <c r="U88" s="31"/>
       <c r="V88" s="39"/>
       <c r="W88" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="89" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7723,7 +7726,7 @@
       <c r="U89" s="31"/>
       <c r="V89" s="39"/>
       <c r="W89" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="90" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7760,7 +7763,7 @@
       <c r="U90" s="31"/>
       <c r="V90" s="39"/>
       <c r="W90" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="91" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7797,7 +7800,7 @@
       <c r="U91" s="31"/>
       <c r="V91" s="39"/>
       <c r="W91" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="92" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7834,7 +7837,7 @@
       <c r="U92" s="31"/>
       <c r="V92" s="39"/>
       <c r="W92" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="93" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7871,7 +7874,7 @@
       <c r="U93" s="31"/>
       <c r="V93" s="39"/>
       <c r="W93" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="94" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7908,7 +7911,7 @@
       <c r="U94" s="31"/>
       <c r="V94" s="39"/>
       <c r="W94" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="95" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7945,7 +7948,7 @@
       <c r="U95" s="31"/>
       <c r="V95" s="39"/>
       <c r="W95" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="96" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -7982,7 +7985,7 @@
       <c r="U96" s="31"/>
       <c r="V96" s="39"/>
       <c r="W96" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="97" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8019,7 +8022,7 @@
       <c r="U97" s="31"/>
       <c r="V97" s="39"/>
       <c r="W97" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="98" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8056,7 +8059,7 @@
       <c r="U98" s="31"/>
       <c r="V98" s="39"/>
       <c r="W98" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="99" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8093,7 +8096,7 @@
       <c r="U99" s="31"/>
       <c r="V99" s="39"/>
       <c r="W99" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="100" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8130,7 +8133,7 @@
       <c r="U100" s="31"/>
       <c r="V100" s="39"/>
       <c r="W100" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="101" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8167,7 +8170,7 @@
       <c r="U101" s="31"/>
       <c r="V101" s="39"/>
       <c r="W101" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="102" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8204,7 +8207,7 @@
       <c r="U102" s="31"/>
       <c r="V102" s="39"/>
       <c r="W102" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="103" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8241,7 +8244,7 @@
       <c r="U103" s="31"/>
       <c r="V103" s="39"/>
       <c r="W103" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="104" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8278,7 +8281,7 @@
       <c r="U104" s="31"/>
       <c r="V104" s="39"/>
       <c r="W104" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="105" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8315,7 +8318,7 @@
       <c r="U105" s="31"/>
       <c r="V105" s="39"/>
       <c r="W105" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="106" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8352,7 +8355,7 @@
       <c r="U106" s="31"/>
       <c r="V106" s="39"/>
       <c r="W106" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="107" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8389,7 +8392,7 @@
       <c r="U107" s="31"/>
       <c r="V107" s="39"/>
       <c r="W107" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="108" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8426,7 +8429,7 @@
       <c r="U108" s="31"/>
       <c r="V108" s="39"/>
       <c r="W108" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="109" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8463,7 +8466,7 @@
       <c r="U109" s="31"/>
       <c r="V109" s="39"/>
       <c r="W109" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="110" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8500,7 +8503,7 @@
       <c r="U110" s="31"/>
       <c r="V110" s="39"/>
       <c r="W110" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="111" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8537,7 +8540,7 @@
       <c r="U111" s="31"/>
       <c r="V111" s="39"/>
       <c r="W111" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="112" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8574,7 +8577,7 @@
       <c r="U112" s="31"/>
       <c r="V112" s="39"/>
       <c r="W112" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="113" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8611,7 +8614,7 @@
       <c r="U113" s="31"/>
       <c r="V113" s="39"/>
       <c r="W113" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="114" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8648,7 +8651,7 @@
       <c r="U114" s="31"/>
       <c r="V114" s="39"/>
       <c r="W114" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="115" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8685,7 +8688,7 @@
       <c r="U115" s="31"/>
       <c r="V115" s="39"/>
       <c r="W115" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="116" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8722,7 +8725,7 @@
       <c r="U116" s="31"/>
       <c r="V116" s="39"/>
       <c r="W116" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="117" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8759,7 +8762,7 @@
       <c r="U117" s="31"/>
       <c r="V117" s="39"/>
       <c r="W117" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="118" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8796,7 +8799,7 @@
       <c r="U118" s="31"/>
       <c r="V118" s="39"/>
       <c r="W118" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="119" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8833,7 +8836,7 @@
       <c r="U119" s="31"/>
       <c r="V119" s="39"/>
       <c r="W119" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="120" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8870,7 +8873,7 @@
       <c r="U120" s="31"/>
       <c r="V120" s="39"/>
       <c r="W120" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="121" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8907,7 +8910,7 @@
       <c r="U121" s="31"/>
       <c r="V121" s="39"/>
       <c r="W121" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="122" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8944,7 +8947,7 @@
       <c r="U122" s="31"/>
       <c r="V122" s="39"/>
       <c r="W122" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="123" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -8981,7 +8984,7 @@
       <c r="U123" s="31"/>
       <c r="V123" s="39"/>
       <c r="W123" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="124" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9018,7 +9021,7 @@
       <c r="U124" s="31"/>
       <c r="V124" s="39"/>
       <c r="W124" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="125" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9055,7 +9058,7 @@
       <c r="U125" s="31"/>
       <c r="V125" s="39"/>
       <c r="W125" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="126" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9092,7 +9095,7 @@
       <c r="U126" s="31"/>
       <c r="V126" s="39"/>
       <c r="W126" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="127" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9129,7 +9132,7 @@
       <c r="U127" s="31"/>
       <c r="V127" s="39"/>
       <c r="W127" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="128" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9166,7 +9169,7 @@
       <c r="U128" s="31"/>
       <c r="V128" s="39"/>
       <c r="W128" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="129" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9203,7 +9206,7 @@
       <c r="U129" s="31"/>
       <c r="V129" s="39"/>
       <c r="W129" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="130" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9240,7 +9243,7 @@
       <c r="U130" s="31"/>
       <c r="V130" s="39"/>
       <c r="W130" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="131" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9277,7 +9280,7 @@
       <c r="U131" s="31"/>
       <c r="V131" s="39"/>
       <c r="W131" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="132" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9314,7 +9317,7 @@
       <c r="U132" s="31"/>
       <c r="V132" s="39"/>
       <c r="W132" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="133" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9351,7 +9354,7 @@
       <c r="U133" s="31"/>
       <c r="V133" s="39"/>
       <c r="W133" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="134" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9388,7 +9391,7 @@
       <c r="U134" s="31"/>
       <c r="V134" s="39"/>
       <c r="W134" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="135" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9425,7 +9428,7 @@
       <c r="U135" s="31"/>
       <c r="V135" s="39"/>
       <c r="W135" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="136" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9462,7 +9465,7 @@
       <c r="U136" s="31"/>
       <c r="V136" s="39"/>
       <c r="W136" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="137" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9499,7 +9502,7 @@
       <c r="U137" s="31"/>
       <c r="V137" s="39"/>
       <c r="W137" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="138" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9536,7 +9539,7 @@
       <c r="U138" s="31"/>
       <c r="V138" s="39"/>
       <c r="W138" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="139" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9573,7 +9576,7 @@
       <c r="U139" s="31"/>
       <c r="V139" s="39"/>
       <c r="W139" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="140" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9610,7 +9613,7 @@
       <c r="U140" s="31"/>
       <c r="V140" s="39"/>
       <c r="W140" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="141" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9647,7 +9650,7 @@
       <c r="U141" s="31"/>
       <c r="V141" s="39"/>
       <c r="W141" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="142" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9684,7 +9687,7 @@
       <c r="U142" s="31"/>
       <c r="V142" s="39"/>
       <c r="W142" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="143" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9721,7 +9724,7 @@
       <c r="U143" s="31"/>
       <c r="V143" s="39"/>
       <c r="W143" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="144" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9758,7 +9761,7 @@
       <c r="U144" s="31"/>
       <c r="V144" s="39"/>
       <c r="W144" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="145" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9795,7 +9798,7 @@
       <c r="U145" s="31"/>
       <c r="V145" s="39"/>
       <c r="W145" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="146" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9832,7 +9835,7 @@
       <c r="U146" s="31"/>
       <c r="V146" s="39"/>
       <c r="W146" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="147" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9869,7 +9872,7 @@
       <c r="U147" s="31"/>
       <c r="V147" s="39"/>
       <c r="W147" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="148" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9906,7 +9909,7 @@
       <c r="U148" s="31"/>
       <c r="V148" s="39"/>
       <c r="W148" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="149" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9943,7 +9946,7 @@
       <c r="U149" s="31"/>
       <c r="V149" s="39"/>
       <c r="W149" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="150" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -9980,7 +9983,7 @@
       <c r="U150" s="31"/>
       <c r="V150" s="39"/>
       <c r="W150" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="151" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10017,7 +10020,7 @@
       <c r="U151" s="31"/>
       <c r="V151" s="39"/>
       <c r="W151" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="152" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10054,7 +10057,7 @@
       <c r="U152" s="31"/>
       <c r="V152" s="39"/>
       <c r="W152" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="153" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10091,7 +10094,7 @@
       <c r="U153" s="31"/>
       <c r="V153" s="39"/>
       <c r="W153" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="154" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10128,7 +10131,7 @@
       <c r="U154" s="31"/>
       <c r="V154" s="39"/>
       <c r="W154" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="155" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10165,7 +10168,7 @@
       <c r="U155" s="31"/>
       <c r="V155" s="39"/>
       <c r="W155" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="156" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10202,7 +10205,7 @@
       <c r="U156" s="31"/>
       <c r="V156" s="39"/>
       <c r="W156" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="157" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10239,7 +10242,7 @@
       <c r="U157" s="31"/>
       <c r="V157" s="39"/>
       <c r="W157" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="158" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10276,7 +10279,7 @@
       <c r="U158" s="31"/>
       <c r="V158" s="39"/>
       <c r="W158" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="159" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10313,7 +10316,7 @@
       <c r="U159" s="31"/>
       <c r="V159" s="39"/>
       <c r="W159" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="160" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10350,7 +10353,7 @@
       <c r="U160" s="31"/>
       <c r="V160" s="39"/>
       <c r="W160" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="161" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10387,7 +10390,7 @@
       <c r="U161" s="31"/>
       <c r="V161" s="39"/>
       <c r="W161" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="162" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10424,7 +10427,7 @@
       <c r="U162" s="31"/>
       <c r="V162" s="39"/>
       <c r="W162" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="163" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10461,7 +10464,7 @@
       <c r="U163" s="31"/>
       <c r="V163" s="39"/>
       <c r="W163" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="164" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10498,7 +10501,7 @@
       <c r="U164" s="31"/>
       <c r="V164" s="39"/>
       <c r="W164" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="165" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10535,7 +10538,7 @@
       <c r="U165" s="31"/>
       <c r="V165" s="39"/>
       <c r="W165" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="166" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10572,7 +10575,7 @@
       <c r="U166" s="31"/>
       <c r="V166" s="39"/>
       <c r="W166" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="167" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10609,7 +10612,7 @@
       <c r="U167" s="31"/>
       <c r="V167" s="39"/>
       <c r="W167" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="168" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10646,7 +10649,7 @@
       <c r="U168" s="31"/>
       <c r="V168" s="39"/>
       <c r="W168" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="169" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10683,7 +10686,7 @@
       <c r="U169" s="31"/>
       <c r="V169" s="39"/>
       <c r="W169" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="170" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10720,7 +10723,7 @@
       <c r="U170" s="31"/>
       <c r="V170" s="39"/>
       <c r="W170" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="171" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10757,7 +10760,7 @@
       <c r="U171" s="31"/>
       <c r="V171" s="39"/>
       <c r="W171" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="172" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10794,7 +10797,7 @@
       <c r="U172" s="31"/>
       <c r="V172" s="39"/>
       <c r="W172" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="173" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10831,7 +10834,7 @@
       <c r="U173" s="31"/>
       <c r="V173" s="39"/>
       <c r="W173" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="174" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10868,7 +10871,7 @@
       <c r="U174" s="31"/>
       <c r="V174" s="39"/>
       <c r="W174" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="175" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10905,7 +10908,7 @@
       <c r="U175" s="31"/>
       <c r="V175" s="39"/>
       <c r="W175" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="176" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10942,7 +10945,7 @@
       <c r="U176" s="31"/>
       <c r="V176" s="39"/>
       <c r="W176" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="177" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -10979,7 +10982,7 @@
       <c r="U177" s="31"/>
       <c r="V177" s="39"/>
       <c r="W177" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="178" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11016,7 +11019,7 @@
       <c r="U178" s="31"/>
       <c r="V178" s="39"/>
       <c r="W178" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="179" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11053,7 +11056,7 @@
       <c r="U179" s="31"/>
       <c r="V179" s="39"/>
       <c r="W179" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="180" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11090,7 +11093,7 @@
       <c r="U180" s="31"/>
       <c r="V180" s="39"/>
       <c r="W180" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="181" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11127,7 +11130,7 @@
       <c r="U181" s="31"/>
       <c r="V181" s="39"/>
       <c r="W181" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="182" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11164,7 +11167,7 @@
       <c r="U182" s="31"/>
       <c r="V182" s="39"/>
       <c r="W182" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="183" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11201,7 +11204,7 @@
       <c r="U183" s="31"/>
       <c r="V183" s="39"/>
       <c r="W183" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="184" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11238,7 +11241,7 @@
       <c r="U184" s="31"/>
       <c r="V184" s="39"/>
       <c r="W184" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="185" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11275,7 +11278,7 @@
       <c r="U185" s="31"/>
       <c r="V185" s="39"/>
       <c r="W185" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="186" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11312,7 +11315,7 @@
       <c r="U186" s="31"/>
       <c r="V186" s="39"/>
       <c r="W186" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="187" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11349,7 +11352,7 @@
       <c r="U187" s="31"/>
       <c r="V187" s="39"/>
       <c r="W187" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="188" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11386,7 +11389,7 @@
       <c r="U188" s="31"/>
       <c r="V188" s="39"/>
       <c r="W188" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="189" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11423,7 +11426,7 @@
       <c r="U189" s="31"/>
       <c r="V189" s="39"/>
       <c r="W189" s="45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="190" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11447,37 +11450,37 @@
       <c r="H190" s="30"/>
       <c r="I190" s="30"/>
       <c r="J190" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K190" s="34" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="L190" s="34"/>
       <c r="M190" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N190" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O190" s="34"/>
       <c r="P190" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q190" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R190" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S190" s="34"/>
       <c r="T190" s="34"/>
       <c r="U190" s="31"/>
       <c r="V190" s="39"/>
       <c r="W190" s="45" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="191" spans="1:23" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="191" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="14">
         <v>368</v>
       </c>
@@ -11500,38 +11503,38 @@
         <v>45593.476770833302</v>
       </c>
       <c r="H191" s="30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I191" s="30" t="s">
+        <v>497</v>
+      </c>
+      <c r="J191" s="34" t="s">
         <v>499</v>
-      </c>
-      <c r="J191" s="34" t="s">
-        <v>501</v>
       </c>
       <c r="K191" s="34"/>
       <c r="L191" s="34"/>
       <c r="M191" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N191" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O191" s="34"/>
       <c r="P191" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q191" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R191" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S191" s="34"/>
       <c r="T191" s="34"/>
       <c r="U191" s="31"/>
       <c r="V191" s="39"/>
       <c r="W191" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="192" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11568,7 +11571,7 @@
       <c r="U192" s="31"/>
       <c r="V192" s="39"/>
       <c r="W192" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="193" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11605,7 +11608,7 @@
       <c r="U193" s="31"/>
       <c r="V193" s="39"/>
       <c r="W193" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="194" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11642,7 +11645,7 @@
       <c r="U194" s="31"/>
       <c r="V194" s="39"/>
       <c r="W194" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="195" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11679,7 +11682,7 @@
       <c r="U195" s="31"/>
       <c r="V195" s="39"/>
       <c r="W195" s="45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="196" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -11716,7 +11719,7 @@
       <c r="U196" s="31"/>
       <c r="V196" s="39"/>
       <c r="W196" s="46" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="197" spans="1:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11740,34 +11743,34 @@
       <c r="H197" s="32"/>
       <c r="I197" s="32"/>
       <c r="J197" s="35" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K197" s="35" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="L197" s="35"/>
       <c r="M197" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N197" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O197" s="35"/>
       <c r="P197" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="Q197" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="R197" s="34" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S197" s="35"/>
       <c r="T197" s="35"/>
       <c r="U197" s="37"/>
       <c r="V197" s="40"/>
       <c r="W197" s="47" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="198" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -11804,7 +11807,7 @@
       <c r="U198" s="38"/>
       <c r="V198" s="41"/>
       <c r="W198" s="48" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="199" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -11841,7 +11844,7 @@
       <c r="U199" s="38"/>
       <c r="V199" s="41"/>
       <c r="W199" s="48" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="200" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -11878,7 +11881,7 @@
       <c r="U200" s="38"/>
       <c r="V200" s="41"/>
       <c r="W200" s="48" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="201" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -11915,7 +11918,7 @@
       <c r="U201" s="38"/>
       <c r="V201" s="41"/>
       <c r="W201" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="202" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -11952,7 +11955,7 @@
       <c r="U202" s="38"/>
       <c r="V202" s="41"/>
       <c r="W202" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="203" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -11989,7 +11992,7 @@
       <c r="U203" s="38"/>
       <c r="V203" s="41"/>
       <c r="W203" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="204" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12026,7 +12029,7 @@
       <c r="U204" s="38"/>
       <c r="V204" s="41"/>
       <c r="W204" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="205" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12063,7 +12066,7 @@
       <c r="U205" s="38"/>
       <c r="V205" s="41"/>
       <c r="W205" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="206" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12100,7 +12103,7 @@
       <c r="U206" s="38"/>
       <c r="V206" s="41"/>
       <c r="W206" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="207" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12137,7 +12140,7 @@
       <c r="U207" s="38"/>
       <c r="V207" s="41"/>
       <c r="W207" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="208" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12174,7 +12177,7 @@
       <c r="U208" s="38"/>
       <c r="V208" s="41"/>
       <c r="W208" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="209" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12211,7 +12214,7 @@
       <c r="U209" s="38"/>
       <c r="V209" s="41"/>
       <c r="W209" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="210" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12248,7 +12251,7 @@
       <c r="U210" s="38"/>
       <c r="V210" s="41"/>
       <c r="W210" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="211" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12285,7 +12288,7 @@
       <c r="U211" s="38"/>
       <c r="V211" s="41"/>
       <c r="W211" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="212" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12322,7 +12325,7 @@
       <c r="U212" s="38"/>
       <c r="V212" s="41"/>
       <c r="W212" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="213" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12359,7 +12362,7 @@
       <c r="U213" s="38"/>
       <c r="V213" s="41"/>
       <c r="W213" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="214" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12396,7 +12399,7 @@
       <c r="U214" s="38"/>
       <c r="V214" s="41"/>
       <c r="W214" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="215" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12433,7 +12436,7 @@
       <c r="U215" s="38"/>
       <c r="V215" s="41"/>
       <c r="W215" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="216" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12470,7 +12473,7 @@
       <c r="U216" s="38"/>
       <c r="V216" s="41"/>
       <c r="W216" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="217" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12507,7 +12510,7 @@
       <c r="U217" s="38"/>
       <c r="V217" s="41"/>
       <c r="W217" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="218" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12544,7 +12547,7 @@
       <c r="U218" s="38"/>
       <c r="V218" s="41"/>
       <c r="W218" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="219" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12581,7 +12584,7 @@
       <c r="U219" s="38"/>
       <c r="V219" s="41"/>
       <c r="W219" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="220" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12618,7 +12621,7 @@
       <c r="U220" s="37"/>
       <c r="V220" s="42"/>
       <c r="W220" s="46" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="221" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12655,7 +12658,7 @@
       <c r="U221" s="38"/>
       <c r="V221" s="41"/>
       <c r="W221" s="48" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="222" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12692,7 +12695,7 @@
       <c r="U222" s="38"/>
       <c r="V222" s="41"/>
       <c r="W222" s="48" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="223" spans="1:23" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12729,7 +12732,7 @@
       <c r="U223" s="38"/>
       <c r="V223" s="41"/>
       <c r="W223" s="48" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="224" spans="1:23" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12766,7 +12769,7 @@
       <c r="U224" s="37"/>
       <c r="V224" s="42"/>
       <c r="W224" s="46" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="225" spans="1:23" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12803,7 +12806,7 @@
       <c r="U225" s="38"/>
       <c r="V225" s="41"/>
       <c r="W225" s="48" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="226" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17402,11 +17405,6 @@
     <filterColumn colId="2">
       <filters>
         <filter val="LAB"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="NO"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -17459,42 +17457,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -17524,22 +17522,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17547,13 +17545,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="51" t="s">
+        <v>525</v>
+      </c>
+      <c r="C2" s="53" t="s">
         <v>527</v>
       </c>
-      <c r="C2" s="53" t="s">
-        <v>529</v>
-      </c>
       <c r="D2" s="53" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17561,13 +17559,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17575,13 +17573,13 @@
         <v>34</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C4" s="53">
         <v>446.447</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17589,13 +17587,13 @@
         <v>30</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17603,13 +17601,13 @@
         <v>31</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -17617,13 +17615,13 @@
         <v>32</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -17631,13 +17629,13 @@
         <v>35</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -17645,27 +17643,27 @@
         <v>33</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17673,13 +17671,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18653,26 +18651,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>